<commit_message>
Fixes class to import dependency and removed GDD results
</commit_message>
<xml_diff>
--- a/stats/chart_2_b.xlsx
+++ b/stats/chart_2_b.xlsx
@@ -8,21 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubo9\Desktop\Workspace\ddminj\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A732A5B2-6828-46D5-BAF3-E9D219CD7F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06871C96-658A-46AD-B6FD-F2F8D763A655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{76C4E7CE-BBFA-4642-BC60-85888EE16FB5}"/>
+    <workbookView xWindow="-28920" yWindow="3315" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3" xr2:uid="{76C4E7CE-BBFA-4642-BC60-85888EE16FB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
     <sheet name="Template" sheetId="1" r:id="rId2"/>
-    <sheet name="GDDrec_chart_2_b_20230615_11275" sheetId="3" r:id="rId3"/>
-    <sheet name="HDDrec_chart_2_b_20230615_15281" sheetId="4" r:id="rId4"/>
-    <sheet name="GDD_chart_2_b_20230615_192837" sheetId="5" r:id="rId5"/>
-    <sheet name="HDD_chart_2_b_20230615_232859" sheetId="6" r:id="rId6"/>
-    <sheet name="CodeLine__2__20230616_032944" sheetId="7" r:id="rId7"/>
+    <sheet name="HDDrec_chart_2_b_20230615_15281" sheetId="4" r:id="rId3"/>
+    <sheet name="HDD_chart_2_b_20230615_232859" sheetId="6" r:id="rId4"/>
+    <sheet name="CodeLine__2__20230616_032944" sheetId="7" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="59">
   <si>
     <t>Execution Time (ms)</t>
   </si>
@@ -185,9 +183,6 @@
     <t>Average run size</t>
   </si>
   <si>
-    <t>0-1</t>
-  </si>
-  <si>
     <t>0-0</t>
   </si>
   <si>
@@ -215,13 +210,7 @@
     <t>chart_2_b</t>
   </si>
   <si>
-    <t>GDDrec</t>
-  </si>
-  <si>
     <t>HDDrec</t>
-  </si>
-  <si>
-    <t>GDD</t>
   </si>
   <si>
     <t>HDD</t>
@@ -1213,373 +1202,6 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>GDDrec_chart_2_b_20230615_11275!$J$32:$J$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>11716</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11716</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>GDDrec_chart_2_b_20230615_11275!$F$32:$F$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>393931</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>393931</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-900C-4D1E-891F-DC85F22D8CAA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1714316624"/>
-        <c:axId val="1714318064"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1714316624"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t># compiler calls</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1714318064"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1714318064"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t># fragments</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1714316624"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t># of fragments after # of compiler calls</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]Template!$F$31</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total Result</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
               <c:f>HDDrec_chart_2_b_20230615_15281!$J$32:$J$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1846,374 +1468,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t># of fragments after # of compiler calls</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]Template!$F$31</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total Result</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>GDD_chart_2_b_20230615_192837!$J$32:$J$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>12057</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12057</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>GDD_chart_2_b_20230615_192837!$F$32:$F$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>394944</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>394944</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-096D-42DB-8714-9E89ECB92069}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1714316624"/>
-        <c:axId val="1714318064"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1714316624"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t># compiler calls</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1714318064"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1714318064"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t># fragments</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1714316624"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2574,7 +1829,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3584,7 +2839,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE1B4AC3-515D-4023-861C-180A03C0B28C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C1C7914-CFD9-4C3A-BB50-AC8AD9434E63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3627,7 +2882,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C1C7914-CFD9-4C3A-BB50-AC8AD9434E63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{765544E9-A523-46C8-89A0-C592BDEC443F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3651,92 +2906,6 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBF61B65-CE17-420C-BBDA-A87881191A7F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{765544E9-A523-46C8-89A0-C592BDEC443F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4429,427 +3598,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCFA675F-C4E1-4B58-BDDD-840F3A31B999}">
-  <dimension ref="A1:M33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20">
-        <v>407987</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20">
-        <f>COUNTA(A32:A33)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <v>6838600</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21">
-        <f>B27/D20</f>
-        <v>5858</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22">
-        <v>227306</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="4">
-        <f>(B20-B23)/B20</f>
-        <v>3.4452078129940417E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23">
-        <v>393931</v>
-      </c>
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="4">
-        <f>D22/D20</f>
-        <v>1.7226039064970208E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24">
-        <v>3026209</v>
-      </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" t="str">
-        <f>TEXT(B26/86400000,"hh:mm:ss.000")</f>
-        <v>04:00:09.572</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25">
-        <v>108815</v>
-      </c>
-      <c r="C25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25">
-        <f>AVERAGE(B32:B33)</f>
-        <v>332</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>14409572</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27">
-        <v>11716</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32">
-        <v>654</v>
-      </c>
-      <c r="C32">
-        <v>611</v>
-      </c>
-      <c r="D32">
-        <f>B32-C32</f>
-        <v>43</v>
-      </c>
-      <c r="E32">
-        <v>407987</v>
-      </c>
-      <c r="F32">
-        <v>393931</v>
-      </c>
-      <c r="G32">
-        <f>E32-F32</f>
-        <v>14056</v>
-      </c>
-      <c r="H32">
-        <v>11716</v>
-      </c>
-      <c r="I32">
-        <v>87</v>
-      </c>
-      <c r="J32">
-        <f>SUM($H$32:H32)</f>
-        <v>11716</v>
-      </c>
-      <c r="K32">
-        <f>SUM($I$32:I32)</f>
-        <v>87</v>
-      </c>
-      <c r="L32">
-        <v>13754400</v>
-      </c>
-      <c r="M32">
-        <v>14408143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33">
-        <v>10</v>
-      </c>
-      <c r="C33">
-        <v>10</v>
-      </c>
-      <c r="D33">
-        <f>B33-C33</f>
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>393931</v>
-      </c>
-      <c r="F33">
-        <v>393931</v>
-      </c>
-      <c r="G33">
-        <f>E33-F33</f>
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <f>SUM($H$32:H33)</f>
-        <v>11716</v>
-      </c>
-      <c r="K33">
-        <f>SUM($I$32:I33)</f>
-        <v>87</v>
-      </c>
-      <c r="L33">
-        <v>103</v>
-      </c>
-      <c r="M33">
-        <v>14408246</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A49570-398C-4652-84C0-3FF80543AC47}">
   <dimension ref="A1:M32"/>
   <sheetViews>
@@ -4874,13 +3622,13 @@
         <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4896,7 +3644,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4904,7 +3652,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4912,7 +3660,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4920,7 +3668,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4928,7 +3676,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4936,7 +3684,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4944,7 +3692,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5176,7 +3924,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32">
         <v>654</v>
@@ -5225,12 +3973,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06AE9C92-F74B-4105-96E8-50A8AF1FC73A}">
-  <dimension ref="A1:M33"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B5D292-8F72-48C7-991B-E28B7C422755}">
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5250,13 +3998,13 @@
         <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5272,7 +4020,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5280,7 +4028,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5288,7 +4036,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5296,7 +4044,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5304,7 +4052,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5312,7 +4060,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5320,7 +4068,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5398,14 +4146,14 @@
         <v>6</v>
       </c>
       <c r="B20">
-        <v>407987</v>
+        <v>408643</v>
       </c>
       <c r="C20" t="s">
         <v>35</v>
       </c>
       <c r="D20">
-        <f>COUNTA(A32:A33)</f>
-        <v>2</v>
+        <f>COUNTA(A32:A32)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -5420,7 +4168,7 @@
       </c>
       <c r="D21">
         <f>B27/D20</f>
-        <v>6028.5</v>
+        <v>5752</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -5435,7 +4183,7 @@
       </c>
       <c r="D22" s="4">
         <f>(B20-B23)/B20</f>
-        <v>3.1969155879966765E-2</v>
+        <v>2.850409770875801E-2</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -5443,14 +4191,14 @@
         <v>7</v>
       </c>
       <c r="B23">
-        <v>394944</v>
+        <v>396995</v>
       </c>
       <c r="C23" t="s">
         <v>44</v>
       </c>
       <c r="D23" s="4">
         <f>D22/D20</f>
-        <v>1.5984577939983383E-2</v>
+        <v>2.850409770875801E-2</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -5458,14 +4206,14 @@
         <v>3</v>
       </c>
       <c r="B24">
-        <v>3033616</v>
+        <v>3044039</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
       </c>
       <c r="D24" t="str">
         <f>TEXT(B26/86400000,"hh:mm:ss.000")</f>
-        <v>04:00:09.141</v>
+        <v>04:00:32.171</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -5473,14 +4221,14 @@
         <v>4</v>
       </c>
       <c r="B25">
-        <v>109042</v>
+        <v>109471</v>
       </c>
       <c r="C25" t="s">
         <v>45</v>
       </c>
       <c r="D25">
-        <f>AVERAGE(B32:B33)</f>
-        <v>3671</v>
+        <f>AVERAGE(B32:B32)</f>
+        <v>654</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -5488,7 +4236,7 @@
         <v>0</v>
       </c>
       <c r="B26">
-        <v>14409141</v>
+        <v>14432171</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -5496,7 +4244,7 @@
         <v>8</v>
       </c>
       <c r="B27">
-        <v>12057</v>
+        <v>5752</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -5504,7 +4252,7 @@
         <v>34</v>
       </c>
       <c r="B28">
-        <v>101</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -5552,92 +4300,47 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32">
         <v>654</v>
       </c>
       <c r="C32">
-        <v>614</v>
+        <v>623</v>
       </c>
       <c r="D32">
         <f>B32-C32</f>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E32">
-        <v>407987</v>
+        <v>408643</v>
       </c>
       <c r="F32">
-        <v>394944</v>
+        <v>396995</v>
       </c>
       <c r="G32">
         <f>E32-F32</f>
-        <v>13043</v>
+        <v>11648</v>
       </c>
       <c r="H32">
-        <v>12057</v>
+        <v>5752</v>
       </c>
       <c r="I32">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="J32">
         <f>SUM($H$32:H32)</f>
-        <v>12057</v>
+        <v>5752</v>
       </c>
       <c r="K32">
         <f>SUM($I$32:I32)</f>
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="L32">
-        <v>13800833</v>
+        <v>14417275</v>
       </c>
       <c r="M32">
-        <v>14407067</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33">
-        <v>6688</v>
-      </c>
-      <c r="C33">
-        <v>6688</v>
-      </c>
-      <c r="D33">
-        <f>B33-C33</f>
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>394944</v>
-      </c>
-      <c r="F33">
-        <v>394944</v>
-      </c>
-      <c r="G33">
-        <f>E33-F33</f>
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <f>SUM($H$32:H33)</f>
-        <v>12057</v>
-      </c>
-      <c r="K33">
-        <f>SUM($I$32:I33)</f>
-        <v>101</v>
-      </c>
-      <c r="L33">
-        <v>1194</v>
-      </c>
-      <c r="M33">
-        <v>14408261</v>
+        <v>14430983</v>
       </c>
     </row>
   </sheetData>
@@ -5646,387 +4349,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B5D292-8F72-48C7-991B-E28B7C422755}">
-  <dimension ref="A1:M32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20">
-        <v>408643</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20">
-        <f>COUNTA(A32:A32)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <v>6838600</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21">
-        <f>B27/D20</f>
-        <v>5752</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22">
-        <v>227306</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="4">
-        <f>(B20-B23)/B20</f>
-        <v>2.850409770875801E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23">
-        <v>396995</v>
-      </c>
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="4">
-        <f>D22/D20</f>
-        <v>2.850409770875801E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24">
-        <v>3044039</v>
-      </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" t="str">
-        <f>TEXT(B26/86400000,"hh:mm:ss.000")</f>
-        <v>04:00:32.171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25">
-        <v>109471</v>
-      </c>
-      <c r="C25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25">
-        <f>AVERAGE(B32:B32)</f>
-        <v>654</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>14432171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27">
-        <v>5752</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32">
-        <v>654</v>
-      </c>
-      <c r="C32">
-        <v>623</v>
-      </c>
-      <c r="D32">
-        <f>B32-C32</f>
-        <v>31</v>
-      </c>
-      <c r="E32">
-        <v>408643</v>
-      </c>
-      <c r="F32">
-        <v>396995</v>
-      </c>
-      <c r="G32">
-        <f>E32-F32</f>
-        <v>11648</v>
-      </c>
-      <c r="H32">
-        <v>5752</v>
-      </c>
-      <c r="I32">
-        <v>48</v>
-      </c>
-      <c r="J32">
-        <f>SUM($H$32:H32)</f>
-        <v>5752</v>
-      </c>
-      <c r="K32">
-        <f>SUM($I$32:I32)</f>
-        <v>48</v>
-      </c>
-      <c r="L32">
-        <v>14417275</v>
-      </c>
-      <c r="M32">
-        <v>14430983</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3082D4C-68F7-4C55-A748-D351690B0099}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -6047,13 +4374,13 @@
         <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6069,7 +4396,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6077,7 +4404,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6085,7 +4412,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6093,7 +4420,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6101,7 +4428,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6109,7 +4436,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6117,7 +4444,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6349,7 +4676,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B32">
         <v>227306</v>

</xml_diff>